<commit_message>
Remove pin headers from button panel.
</commit_message>
<xml_diff>
--- a/CAM_Outputs/USER_BREAKOUT/BOM/USER_SW_Breakout_CAM_OUTPUT_A6.xlsx
+++ b/CAM_Outputs/USER_BREAKOUT/BOM/USER_SW_Breakout_CAM_OUTPUT_A6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\USER_BREAKOUT\Project Outputs for USER_SW_Breakout\USER_SW_Breakout_UPLOAD_GERBERS_A6\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\CAM_Outputs\USER_BREAKOUT\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Comment</t>
   </si>
@@ -78,21 +78,6 @@
   </si>
   <si>
     <t>C72038</t>
-  </si>
-  <si>
-    <t>WJ15EDGVC-3.5-3P</t>
-  </si>
-  <si>
-    <t>Header,Male Pin,Covered(4 Sided) 3 1 0.138"（3.50mm） 3 P=3.5mm Pluggable System Terminal Block RoHS</t>
-  </si>
-  <si>
-    <t>J25, J26, J27, J28</t>
-  </si>
-  <si>
-    <t>SL_3_50_180G_03</t>
-  </si>
-  <si>
-    <t>C192778</t>
   </si>
   <si>
     <t>2KΩ ±1%</t>
@@ -467,7 +452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -557,40 +544,28 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1">
         <v>7</v>
@@ -598,19 +573,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Update user breakout BOM to address LED forward voltage variation.
</commit_message>
<xml_diff>
--- a/CAM_Outputs/USER_BREAKOUT/BOM/USER_SW_Breakout_CAM_OUTPUT_A6.xlsx
+++ b/CAM_Outputs/USER_BREAKOUT/BOM/USER_SW_Breakout_CAM_OUTPUT_A6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\USER_BREAKOUT\Project Outputs for USER_SW_Breakout\USER_SW_Breakout_UPLOAD_GERBERS_A6\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\CAM_Outputs\USER_BREAKOUT\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,9 +101,6 @@
     <t>Chip resistor</t>
   </si>
   <si>
-    <t>R85, R86, R87, R88, R89, R90, R91</t>
-  </si>
-  <si>
     <t>0603_R</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>C127509</t>
+  </si>
+  <si>
+    <t>R85, R87, R89, R90</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -584,33 +586,33 @@
         <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>

</xml_diff>